<commit_message>
moved traces away from pads, regenerated gerbers
</commit_message>
<xml_diff>
--- a/Keyboard/Project Outputs for Keyboard/BOM/Bill of Materials-Keyboard.xlsx
+++ b/Keyboard/Project Outputs for Keyboard/BOM/Bill of Materials-Keyboard.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\college\osu_keyboard\Keyboard\Project Outputs for Keyboard\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{75511CB1-F43B-43D5-A188-32A942548022}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{31596B3C-6BF0-446A-91B2-6402BA90E70B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="384" yWindow="384" windowWidth="17280" windowHeight="8964" xr2:uid="{79ED5C63-D172-491B-8681-EBBB299F8917}"/>
+    <workbookView xWindow="384" yWindow="384" windowWidth="17280" windowHeight="8964" xr2:uid="{0A3ACCBE-1393-4001-AAD9-D9728B2D8284}"/>
   </bookViews>
   <sheets>
     <sheet name="Bill of Materials-Keyboard" sheetId="1" r:id="rId1"/>
@@ -454,7 +454,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D159DD1D-79BE-45E0-BC2A-A5C7892500D0}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5800359E-BE1F-4018-BFD5-31178DA40885}">
   <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>

</xml_diff>

<commit_message>
cutouts weren't showing up on JLCPCB
</commit_message>
<xml_diff>
--- a/Keyboard/Project Outputs for Keyboard/BOM/Bill of Materials-Keyboard.xlsx
+++ b/Keyboard/Project Outputs for Keyboard/BOM/Bill of Materials-Keyboard.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\college\osu_keyboard\Keyboard\Project Outputs for Keyboard\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{31596B3C-6BF0-446A-91B2-6402BA90E70B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{E4BB84E4-495F-49CE-B2D2-19733DCA54EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="384" yWindow="384" windowWidth="17280" windowHeight="8964" xr2:uid="{0A3ACCBE-1393-4001-AAD9-D9728B2D8284}"/>
+    <workbookView xWindow="2304" yWindow="2304" windowWidth="17280" windowHeight="8964" xr2:uid="{3739F4EB-4B67-4553-AE66-21B0CC21A4AC}"/>
   </bookViews>
   <sheets>
     <sheet name="Bill of Materials-Keyboard" sheetId="1" r:id="rId1"/>
@@ -454,7 +454,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5800359E-BE1F-4018-BFD5-31178DA40885}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{164C633E-34C8-4249-AF3F-27A1EC505E69}">
   <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>

</xml_diff>